<commit_message>
Update sample template file
</commit_message>
<xml_diff>
--- a/uploads/sample_template.xlsx
+++ b/uploads/sample_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khair\Documents\GitHub\repositories\rendr\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khair\Documents\GitHub\repositories\rendr\sample\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DFC76E-01BB-4578-86A9-B7C4FA2F53FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E819E7-27FF-4F9C-AA3F-D11848031F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6030" yWindow="1410" windowWidth="28800" windowHeight="11385" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pension Investment Status" sheetId="3" r:id="rId1"/>
@@ -37,11 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="98">
-  <si>
-    <t>Code</t>
-    <phoneticPr fontId="3"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="117">
   <si>
     <t>Company Name</t>
     <phoneticPr fontId="3"/>
@@ -66,48 +62,6 @@
     <t>zzz</t>
   </si>
   <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>09/30/2021</t>
-  </si>
-  <si>
-    <t>00ABC1111111111</t>
-  </si>
-  <si>
-    <t>ANEWCOMPANY1</t>
-  </si>
-  <si>
-    <t>XY0000000001</t>
-  </si>
-  <si>
-    <t>POLLPOLLOFFSHORE</t>
-  </si>
-  <si>
-    <t>LMB100100101</t>
-  </si>
-  <si>
-    <t>OCEANWAVELP</t>
-  </si>
-  <si>
-    <t>FG120012001</t>
-  </si>
-  <si>
-    <t>JAMESANDCO1221</t>
-  </si>
-  <si>
-    <t>1820MN444221</t>
-  </si>
-  <si>
-    <t>APPLEPIE1010</t>
-  </si>
-  <si>
-    <t>ABC Company</t>
-  </si>
-  <si>
     <t>Accounting Standard(2)</t>
   </si>
   <si>
@@ -120,9 +74,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Total Inflow</t>
-  </si>
-  <si>
     <t>Total Outflow</t>
   </si>
   <si>
@@ -130,9 +81,6 @@
   </si>
   <si>
     <t>Current Month Withdrawal/Deposit</t>
-  </si>
-  <si>
-    <t>Deposit</t>
   </si>
   <si>
     <t>Withdrawal</t>
@@ -180,17 +128,10 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>Allocation</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>Current Month
 Realized Gain/Loss</t>
   </si>
   <si>
-    <t>Goldman Sachs Asset Management Co.</t>
-  </si>
-  <si>
     <t>Record Date(YYYY)(MM)</t>
   </si>
   <si>
@@ -229,130 +170,245 @@
     <t>Off-Balance Sheet Swaps(9)</t>
   </si>
   <si>
+    <t>Shareholder Name</t>
+  </si>
+  <si>
+    <t>Total Redemptions (Includes Interest and Dividend Income)</t>
+  </si>
+  <si>
+    <t>Record Date</t>
+  </si>
+  <si>
+    <t>Additional Notes (Not required in the generated report)</t>
+  </si>
+  <si>
+    <t>Holdings are content of an investment portfolio held by an individudal or an entity.</t>
+  </si>
+  <si>
+    <t>Each portfolio may contain a wide range of investment products such as stocks, bonds, options etc.</t>
+  </si>
+  <si>
+    <t>This holdings report details the investment products behind one of our portfolios.</t>
+  </si>
+  <si>
+    <t>Some of the terminologies used in the report are explained as follows:</t>
+  </si>
+  <si>
+    <t>Market Capitalization</t>
+  </si>
+  <si>
+    <t>Total market value of the related investment products</t>
+  </si>
+  <si>
+    <t>Cash Inflow</t>
+  </si>
+  <si>
+    <t>Cash Outflow</t>
+  </si>
+  <si>
+    <t>Cash transferred out of the portfolio</t>
+  </si>
+  <si>
+    <t>Cash transferred into the portfolio</t>
+  </si>
+  <si>
+    <t>Purchase</t>
+  </si>
+  <si>
+    <t>Buying of investment products</t>
+  </si>
+  <si>
+    <t>Redemption</t>
+  </si>
+  <si>
+    <t>Selling of investment products</t>
+  </si>
+  <si>
+    <t>Amount investor could potentially lose in an investment if the investment fails</t>
+  </si>
+  <si>
+    <t>The mapping of information between the report and the JSON files are described as follows:</t>
+  </si>
+  <si>
+    <t>Client Information (C3:I5)</t>
+  </si>
+  <si>
+    <t>Complex-3-Client_Details.json</t>
+  </si>
+  <si>
+    <t>Total Inflow (J21)</t>
+  </si>
+  <si>
+    <t>Complex-1-Account_Inflow_Details.json</t>
+  </si>
+  <si>
+    <t>Outflow (I22:J23)</t>
+  </si>
+  <si>
+    <t>Complex-2-Account_Outflow_Details.json</t>
+  </si>
+  <si>
+    <t>Withdrawal/Deposit (C21:D24)</t>
+  </si>
+  <si>
+    <t>Complex-4-Account_NAV_Details.json</t>
+  </si>
+  <si>
+    <t>Stock Balance Sheet</t>
+  </si>
+  <si>
+    <t>Complex-5-Syntax_Report.json</t>
+  </si>
+  <si>
+    <t>Complex-6-Asset_Outflow_Details.json</t>
+  </si>
+  <si>
+    <t>Asset Outflow (G9:H13)</t>
+  </si>
+  <si>
+    <t>Asset Inflow (E9:F13)</t>
+  </si>
+  <si>
+    <t>Complex-7-Asset_Inflow_Details.json</t>
+  </si>
+  <si>
+    <t>Other Info (Market Capitalization, Financial Exposure etc)</t>
+  </si>
+  <si>
+    <t>Complex-8-Asset_Inflow_Details.json</t>
+  </si>
+  <si>
+    <t>The Currency Overlay section is left empty intentionally -- this section is hardcoded and is not populated with any information from the JSON; your implementation should allow such configurations.</t>
+  </si>
+  <si>
+    <t>Take note of some cells that contain Excel formulas -- your implementation should account for such inputs.</t>
+  </si>
+  <si>
+    <t>Metric used to evaluate performance of an investment product; ratio between the profit and cost of the investment</t>
+  </si>
+  <si>
+    <t>Return on Investment</t>
+  </si>
+  <si>
+    <t>Report generated should be in .xlsx format.</t>
+  </si>
+  <si>
+    <t>!!v assetCode</t>
+  </si>
+  <si>
+    <t>!!v assetName</t>
+  </si>
+  <si>
+    <t>Deposit</t>
+  </si>
+  <si>
+    <t>Total Inflow</t>
+  </si>
+  <si>
+    <t>Allocation</t>
+  </si>
+  <si>
     <t>Currency Overlay Notional Amount</t>
   </si>
   <si>
-    <t>Shareholder Name</t>
-  </si>
-  <si>
-    <t>Total Redemptions (Includes Interest and Dividend Income)</t>
-  </si>
-  <si>
-    <t>Record Date</t>
-  </si>
-  <si>
-    <t>Additional Notes (Not required in the generated report)</t>
-  </si>
-  <si>
-    <t>Holdings are content of an investment portfolio held by an individudal or an entity.</t>
-  </si>
-  <si>
-    <t>Each portfolio may contain a wide range of investment products such as stocks, bonds, options etc.</t>
-  </si>
-  <si>
-    <t>This holdings report details the investment products behind one of our portfolios.</t>
-  </si>
-  <si>
-    <t>Some of the terminologies used in the report are explained as follows:</t>
-  </si>
-  <si>
-    <t>Market Capitalization</t>
-  </si>
-  <si>
-    <t>Total market value of the related investment products</t>
-  </si>
-  <si>
-    <t>Cash Inflow</t>
-  </si>
-  <si>
-    <t>Cash Outflow</t>
-  </si>
-  <si>
-    <t>Cash transferred out of the portfolio</t>
-  </si>
-  <si>
-    <t>Cash transferred into the portfolio</t>
-  </si>
-  <si>
-    <t>Purchase</t>
-  </si>
-  <si>
-    <t>Buying of investment products</t>
-  </si>
-  <si>
-    <t>Redemption</t>
-  </si>
-  <si>
-    <t>Selling of investment products</t>
-  </si>
-  <si>
-    <t>Amount investor could potentially lose in an investment if the investment fails</t>
-  </si>
-  <si>
-    <t>The mapping of information between the report and the JSON files are described as follows:</t>
-  </si>
-  <si>
-    <t>Client Information (C3:I5)</t>
-  </si>
-  <si>
-    <t>Complex-3-Client_Details.json</t>
-  </si>
-  <si>
-    <t>Total Inflow (J21)</t>
-  </si>
-  <si>
-    <t>Complex-1-Account_Inflow_Details.json</t>
-  </si>
-  <si>
-    <t>Outflow (I22:J23)</t>
-  </si>
-  <si>
-    <t>Complex-2-Account_Outflow_Details.json</t>
-  </si>
-  <si>
-    <t>Withdrawal/Deposit (C21:D24)</t>
-  </si>
-  <si>
-    <t>Complex-4-Account_NAV_Details.json</t>
-  </si>
-  <si>
-    <t>Stock Balance Sheet</t>
-  </si>
-  <si>
-    <t>Complex-5-Syntax_Report.json</t>
-  </si>
-  <si>
-    <t>Complex-6-Asset_Outflow_Details.json</t>
-  </si>
-  <si>
-    <t>Asset Outflow (G9:H13)</t>
-  </si>
-  <si>
-    <t>Asset Inflow (E9:F13)</t>
-  </si>
-  <si>
-    <t>Complex-7-Asset_Inflow_Details.json</t>
-  </si>
-  <si>
-    <t>Other Info (Market Capitalization, Financial Exposure etc)</t>
-  </si>
-  <si>
-    <t>Complex-8-Asset_Inflow_Details.json</t>
-  </si>
-  <si>
-    <t>The Currency Overlay section is left empty intentionally -- this section is hardcoded and is not populated with any information from the JSON; your implementation should allow such configurations.</t>
-  </si>
-  <si>
-    <t>Take note of some cells that contain Excel formulas -- your implementation should account for such inputs.</t>
-  </si>
-  <si>
-    <t>Metric used to evaluate performance of an investment product; ratio between the profit and cost of the investment</t>
-  </si>
-  <si>
-    <t>Return on Investment</t>
-  </si>
-  <si>
-    <t>Report generated should be in .xlsx format.</t>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>##checkInflow</t>
+  </si>
+  <si>
+    <t>##checkOutflow</t>
+  </si>
+  <si>
+    <t>##assetManagerCode1</t>
+  </si>
+  <si>
+    <t>##clientCode1</t>
+  </si>
+  <si>
+    <t>##DateYear</t>
+  </si>
+  <si>
+    <t>##DateMonth</t>
+  </si>
+  <si>
+    <t>ABC Company Ltd.</t>
+  </si>
+  <si>
+    <t>Goldman Sachs Asset Management Co.</t>
+  </si>
+  <si>
+    <t>##assetManagerCode2</t>
+  </si>
+  <si>
+    <t>##netIncreaseDecrease</t>
+  </si>
+  <si>
+    <t>##clientWithdrawal</t>
+  </si>
+  <si>
+    <t>##clientContribution</t>
+  </si>
+  <si>
+    <t>##totalCashOutflow</t>
+  </si>
+  <si>
+    <t>ABC Company</t>
+  </si>
+  <si>
+    <t>##reportingMonth</t>
+  </si>
+  <si>
+    <t>!!v security_cd</t>
+  </si>
+  <si>
+    <t>!!v securityDescription</t>
+  </si>
+  <si>
+    <t>!!v market_value_bs</t>
+  </si>
+  <si>
+    <t>!!v trade_ccy_cd</t>
+  </si>
+  <si>
+    <t>!!v outflow</t>
+  </si>
+  <si>
+    <t>!!v daysOutflow</t>
+  </si>
+  <si>
+    <t>!!v inflow</t>
+  </si>
+  <si>
+    <t>!!v daysInflow</t>
+  </si>
+  <si>
+    <t>!!v previousMonthNAV</t>
+  </si>
+  <si>
+    <t>!!v currentMonthNAV</t>
+  </si>
+  <si>
+    <t>!!v exposure</t>
+  </si>
+  <si>
+    <t>!!v compositionRate</t>
+  </si>
+  <si>
+    <t>Contract Basis/Accrual Basis</t>
+  </si>
+  <si>
+    <t>Operations</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>81(3)0000-0000</t>
+  </si>
+  <si>
+    <t>!!v</t>
+  </si>
+  <si>
+    <t>##totalTransDaysOutflow</t>
   </si>
 </sst>
 </file>
@@ -1574,9 +1630,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="38" fontId="2" fillId="11" borderId="6" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1737,9 +1790,69 @@
     <xf numFmtId="166" fontId="7" fillId="0" borderId="6" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="38" fontId="2" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="38" fontId="2" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1770,62 +1883,26 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="40" fontId="22" fillId="0" borderId="6" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="40" fontId="22" fillId="0" borderId="30" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="40" fontId="22" fillId="0" borderId="31" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="40" fontId="22" fillId="0" borderId="32" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="28" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1836,9 +1913,6 @@
     <xf numFmtId="166" fontId="7" fillId="0" borderId="29" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="22" fillId="0" borderId="6" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="41" fillId="38" borderId="30" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1847,24 +1921,6 @@
     </xf>
     <xf numFmtId="166" fontId="41" fillId="38" borderId="32" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="22" fillId="0" borderId="30" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="22" fillId="0" borderId="31" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="22" fillId="0" borderId="32" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="88">
@@ -2422,8 +2478,8 @@
   </sheetPr>
   <dimension ref="B2:O39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:H3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2446,183 +2502,223 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="27" customHeight="1">
-      <c r="B2" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
+      <c r="B2" s="79" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:15" ht="13.5" customHeight="1" thickBot="1">
       <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="108" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="108"/>
-      <c r="I3" s="5"/>
+      <c r="G3" s="91" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="91"/>
+      <c r="I3" s="5" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="4" spans="2:15" ht="13.5" customHeight="1" thickBot="1">
       <c r="C4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="108" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="108"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="47"/>
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="91" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="91"/>
+      <c r="I4" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="2:15" ht="13.5" customHeight="1" thickBot="1">
       <c r="C5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="72" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="108" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="108"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+        <v>25</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="91" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="91"/>
+      <c r="I5" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="J5" s="37"/>
       <c r="K5" s="9"/>
     </row>
     <row r="6" spans="2:15" ht="14.25" thickBot="1"/>
     <row r="7" spans="2:15" ht="13.5" customHeight="1">
-      <c r="B7" s="99"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="103" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="98" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="98"/>
-      <c r="I7" s="79" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" s="106" t="s">
-        <v>51</v>
+      <c r="B7" s="81"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="85" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="80"/>
+      <c r="I7" s="87" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="89" t="s">
+        <v>32</v>
       </c>
       <c r="K7" s="8"/>
-      <c r="L7" s="91" t="s">
-        <v>41</v>
-      </c>
-      <c r="N7" s="67"/>
+      <c r="L7" s="92" t="s">
+        <v>82</v>
+      </c>
+      <c r="N7" s="66"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="B8" s="101"/>
-      <c r="C8" s="102"/>
-      <c r="D8" s="104"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="86"/>
       <c r="E8" s="13" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="105"/>
-      <c r="J8" s="107"/>
+        <v>8</v>
+      </c>
+      <c r="I8" s="88"/>
+      <c r="J8" s="90"/>
       <c r="K8" s="8"/>
-      <c r="L8" s="92"/>
-    </row>
-    <row r="9" spans="2:15">
-      <c r="B9" s="51"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="55"/>
-      <c r="L9" s="56"/>
-      <c r="O9" s="35"/>
+      <c r="L8" s="93"/>
+    </row>
+    <row r="9" spans="2:15" ht="54">
+      <c r="B9" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="J9" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="L9" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="O9" s="34"/>
     </row>
     <row r="10" spans="2:15">
-      <c r="B10" s="51"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="55"/>
-      <c r="L10" s="56"/>
-      <c r="O10" s="35"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="54"/>
+      <c r="L10" s="55"/>
+      <c r="O10" s="34"/>
     </row>
     <row r="11" spans="2:15">
-      <c r="B11" s="51"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="55"/>
-      <c r="L11" s="56"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="54"/>
+      <c r="L11" s="55"/>
     </row>
     <row r="12" spans="2:15">
-      <c r="B12" s="51"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="55"/>
-      <c r="L12" s="56"/>
-      <c r="O12" s="35"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="54"/>
+      <c r="L12" s="55"/>
+      <c r="O12" s="34"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="B13" s="51"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="55"/>
-      <c r="L13" s="56"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="54"/>
+      <c r="L13" s="55"/>
     </row>
     <row r="14" spans="2:15">
       <c r="B14" s="10"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="25"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
-      <c r="I14" s="25"/>
+      <c r="I14" s="24"/>
       <c r="J14" s="17"/>
       <c r="L14" s="20" t="e">
         <f>J14/J16</f>
@@ -2631,13 +2727,13 @@
     </row>
     <row r="15" spans="2:15">
       <c r="B15" s="10"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="25"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
-      <c r="I15" s="25"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="17"/>
       <c r="L15" s="20" t="e">
         <f>J15/J16</f>
@@ -2646,139 +2742,153 @@
     </row>
     <row r="16" spans="2:15" ht="14.25" thickBot="1">
       <c r="B16" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="27">
+        <v>9</v>
+      </c>
+      <c r="D16" s="26">
         <f>SUM(D9:D15)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="25" t="str">
         <f>+D21</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="57"/>
-      <c r="G16" s="26">
-        <f>+D22+D23</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="57"/>
-      <c r="I16" s="27">
+        <v>##clientContribution</v>
+      </c>
+      <c r="F16" s="56"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="26">
         <f>SUM(I9:I15)</f>
         <v>0</v>
       </c>
-      <c r="J16" s="28">
+      <c r="J16" s="27">
         <f>SUM(J9:J15)</f>
         <v>0</v>
       </c>
-      <c r="L16" s="58"/>
+      <c r="L16" s="57" t="e">
+        <f>SUM(L10:L15)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="17" spans="2:11">
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="2:11">
       <c r="E18" s="8"/>
-      <c r="I18" s="37"/>
+      <c r="I18" s="36"/>
     </row>
     <row r="20" spans="2:11" ht="13.5" customHeight="1" thickBot="1">
-      <c r="B20" s="90" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="90"/>
+      <c r="B20" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="94"/>
       <c r="I20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J20" s="70"/>
+        <v>33</v>
+      </c>
+      <c r="J20" s="69"/>
     </row>
     <row r="21" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B21" s="93" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="94"/>
-      <c r="D21" s="59"/>
+      <c r="B21" s="95" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="96"/>
+      <c r="D21" s="58" t="s">
+        <v>96</v>
+      </c>
       <c r="E21" s="8"/>
       <c r="I21" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="J21" s="60"/>
+        <v>81</v>
+      </c>
+      <c r="J21" s="59" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="22" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B22" s="95" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="96"/>
-      <c r="D22" s="55"/>
+      <c r="B22" s="97" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="98"/>
+      <c r="D22" s="54" t="s">
+        <v>97</v>
+      </c>
       <c r="E22" s="8"/>
       <c r="I22" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J22" s="61"/>
+        <v>10</v>
+      </c>
+      <c r="J22" s="60" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="23" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B23" s="95" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="96"/>
-      <c r="D23" s="55"/>
+      <c r="B23" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="98"/>
+      <c r="D23" s="54" t="s">
+        <v>95</v>
+      </c>
       <c r="I23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="60" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="14.25" thickBot="1">
+      <c r="B24" s="103" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="104"/>
+      <c r="D24" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="62"/>
+      <c r="K24" s="68"/>
+    </row>
+    <row r="27" spans="2:11" ht="14.25" thickBot="1">
+      <c r="B27" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="J23" s="61"/>
-    </row>
-    <row r="24" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B24" s="84" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="85"/>
-      <c r="D24" s="62"/>
-      <c r="I24" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J24" s="63"/>
-      <c r="K24" s="69"/>
-    </row>
-    <row r="27" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B27" s="90" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="90"/>
-      <c r="D27" s="90"/>
-      <c r="E27" s="90"/>
-      <c r="F27" s="90"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="94"/>
+      <c r="F27" s="94"/>
     </row>
     <row r="28" spans="2:11" ht="40.5">
-      <c r="B28" s="86"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="71" t="s">
+      <c r="B28" s="105"/>
+      <c r="C28" s="106"/>
+      <c r="D28" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="87" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="99"/>
+      <c r="I28" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="73" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="14.25" thickBot="1">
+      <c r="B29" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="79" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" s="79"/>
-      <c r="G28" s="79" t="s">
-        <v>42</v>
-      </c>
-      <c r="H28" s="80"/>
-      <c r="I28" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="J28" s="74" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B29" s="88" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="89"/>
+      <c r="C29" s="108"/>
       <c r="D29" s="16"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="81"/>
-      <c r="G29" s="81"/>
-      <c r="H29" s="81"/>
+      <c r="E29" s="100"/>
+      <c r="F29" s="100"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="100"/>
       <c r="I29" s="18">
         <f>E29 - D29</f>
         <v>0</v>
@@ -2789,44 +2899,58 @@
       </c>
     </row>
     <row r="30" spans="2:11" ht="14.25" thickBot="1">
-      <c r="G30" s="69"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="69"/>
+      <c r="G30" s="68"/>
+      <c r="I30" s="68"/>
+      <c r="J30" s="68"/>
     </row>
     <row r="31" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B31" s="82" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="83"/>
+      <c r="B31" s="101" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="102"/>
       <c r="D31" s="22"/>
-      <c r="G31" s="32"/>
+      <c r="G31" s="31"/>
     </row>
     <row r="32" spans="2:11">
-      <c r="G32" s="32"/>
+      <c r="G32" s="31"/>
     </row>
     <row r="33" spans="7:7">
-      <c r="G33" s="32"/>
+      <c r="G33" s="31"/>
     </row>
     <row r="34" spans="7:7">
-      <c r="G34" s="32"/>
+      <c r="G34" s="31"/>
     </row>
     <row r="35" spans="7:7">
-      <c r="G35" s="32"/>
+      <c r="G35" s="31"/>
     </row>
     <row r="36" spans="7:7">
-      <c r="G36" s="32"/>
+      <c r="G36" s="31"/>
     </row>
     <row r="37" spans="7:7">
-      <c r="G37" s="33"/>
+      <c r="G37" s="32"/>
     </row>
     <row r="38" spans="7:7">
-      <c r="G38" s="32"/>
+      <c r="G38" s="31"/>
     </row>
     <row r="39" spans="7:7">
-      <c r="G39" s="34"/>
+      <c r="G39" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:H7"/>
@@ -2837,20 +2961,6 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <phoneticPr fontId="18"/>
   <printOptions horizontalCentered="1"/>
@@ -2869,14 +2979,14 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="2" width="61.125" customWidth="1"/>
-    <col min="3" max="3" width="14.25" style="39" customWidth="1"/>
+    <col min="3" max="3" width="14.25" style="38" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.625" customWidth="1"/>
     <col min="6" max="6" width="14.125" customWidth="1"/>
@@ -2887,160 +2997,132 @@
     </row>
     <row r="2" spans="1:6" ht="14.25" thickBot="1">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="68"/>
+        <v>98</v>
+      </c>
+      <c r="C2" s="67"/>
     </row>
     <row r="3" spans="1:6" ht="14.25" thickBot="1">
-      <c r="A3" s="75" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="68"/>
+      <c r="A3" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="67"/>
     </row>
     <row r="4" spans="1:6" ht="14.25" thickBot="1">
-      <c r="A4" s="76" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="68"/>
+      <c r="A4" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="67"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="C6" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="D6" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="E6" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="F6" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="43" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="65" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="66">
-        <v>1344762582</v>
-      </c>
-      <c r="F7" s="65" t="s">
-        <v>8</v>
+      <c r="A7" s="64" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="65" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="64" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="65" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="66">
-        <v>131622258</v>
-      </c>
-      <c r="F8" s="65" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="64"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="65" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="65" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="66">
-        <v>55714753</v>
-      </c>
-      <c r="F9" s="65" t="s">
-        <v>7</v>
-      </c>
+      <c r="A9" s="64"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="64"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="65" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="65" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="66">
-        <v>93126520</v>
-      </c>
-      <c r="F10" s="65" t="s">
-        <v>7</v>
-      </c>
+      <c r="A10" s="64"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="64"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="65" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="66">
-        <v>1561662185</v>
-      </c>
-      <c r="F11" s="65" t="s">
-        <v>7</v>
-      </c>
+      <c r="A11" s="64"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="64"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="30"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="31"/>
+      <c r="A12" s="29"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="30"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="31"/>
+      <c r="A13" s="29"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="30"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="C14" s="40"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="31"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="29"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="31"/>
+      <c r="A15" s="28"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="C16" s="40"/>
-      <c r="D16" s="29"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="28"/>
     </row>
     <row r="21" spans="5:5">
-      <c r="E21" s="36"/>
+      <c r="E21" s="35"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>
@@ -3057,7 +3139,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+      <selection activeCell="A8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3067,263 +3149,253 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="119" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="121"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="116" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="118"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="116" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="118"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="116" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="118"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="116" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="117"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="118"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="116" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="117"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="118"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="116" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="117"/>
+      <c r="C7" s="117"/>
+      <c r="D7" s="117"/>
+      <c r="E7" s="118"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="110" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="111"/>
+      <c r="C8" s="111"/>
+      <c r="D8" s="111"/>
+      <c r="E8" s="112"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="109" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="109"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="76" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="109" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="109"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="76" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="109" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="109"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="109" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="109"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="109"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="76" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="109" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="109"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="109"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="77" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="109" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="109"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="109"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="109" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="109"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="110" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="111"/>
+      <c r="C16" s="111"/>
+      <c r="D16" s="111"/>
+      <c r="E16" s="112"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="76" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="115"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="109" t="s">
+      <c r="C17" s="109"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="109"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="111"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="109" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="110"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="111"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="109" t="s">
+      <c r="B18" s="109" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="110"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="111"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="109" t="s">
+      <c r="C18" s="109"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="109"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="76" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="109" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="109"/>
+      <c r="D19" s="109"/>
+      <c r="E19" s="109"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="110"/>
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="111"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="109" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="110"/>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="111"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="109" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="110"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="111"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="116" t="s">
+      <c r="B20" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="117"/>
-      <c r="C8" s="117"/>
-      <c r="D8" s="117"/>
-      <c r="E8" s="118"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="77" t="s">
+      <c r="C20" s="114"/>
+      <c r="D20" s="114"/>
+      <c r="E20" s="115"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="112" t="s">
+      <c r="B21" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="112"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="77" t="s">
+      <c r="C21" s="109"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="109"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="109" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="112" t="s">
+      <c r="C22" s="109"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="109"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="109" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="112"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="112"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="77" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="112" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="112"/>
-      <c r="D11" s="112"/>
-      <c r="E11" s="112"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="77" t="s">
+      <c r="C23" s="109"/>
+      <c r="D23" s="109"/>
+      <c r="E23" s="109"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="112" t="s">
+      <c r="B24" s="109" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="112"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="112"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="77" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="112" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="112"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="112"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="78" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="112" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="112"/>
-      <c r="D14" s="112"/>
-      <c r="E14" s="112"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="77" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="112" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="112"/>
-      <c r="D15" s="112"/>
-      <c r="E15" s="112"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="116" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="118"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="77" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="112" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="112"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="77" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="112" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="112"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="112"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="77" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="112" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="112"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="112"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="77" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" s="119" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="120"/>
-      <c r="D20" s="120"/>
-      <c r="E20" s="121"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="77" t="s">
-        <v>85</v>
-      </c>
-      <c r="B21" s="112" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="112"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="112"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="77" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="112" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="112"/>
-      <c r="D22" s="112"/>
-      <c r="E22" s="112"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="77" t="s">
-        <v>89</v>
-      </c>
-      <c r="B23" s="112" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="112"/>
-      <c r="D23" s="112"/>
-      <c r="E23" s="112"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="78" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24" s="112" t="s">
-        <v>92</v>
-      </c>
-      <c r="C24" s="112"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="112"/>
+      <c r="C24" s="109"/>
+      <c r="D24" s="109"/>
+      <c r="E24" s="109"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="B18:E18"/>
@@ -3338,27 +3410,22 @@
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008CDC787A71DDF645B3B1EC4B4C087709" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfcc5dabae62faba7569d214b4f3e22c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -3472,10 +3539,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FA689A5-2DDE-4193-801A-F36D3E40FA78}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{835BF43D-5F5B-4A92-8B6A-74ACA0EB3617}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3496,17 +3586,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{835BF43D-5F5B-4A92-8B6A-74ACA0EB3617}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FA689A5-2DDE-4193-801A-F36D3E40FA78}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>